<commit_message>
Removed unnecessary code and continued improving the loging process
</commit_message>
<xml_diff>
--- a/DataLoginFolder/dataLogin.xlsx
+++ b/DataLoginFolder/dataLogin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\eclipse-workspace\SwagLabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\eclipse-workspace\SwagLabs\DataLoginFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFEB6680-AACC-4EC9-B27D-3EF2DC03BEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EE7FE0-FB9A-4A08-A0B1-1F69A993750B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{9DE631A4-C63C-460A-AE8C-CB17A0AD8551}"/>
   </bookViews>
@@ -20,16 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -40,22 +30,22 @@
     <t>standard_user</t>
   </si>
   <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
     <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
   </si>
 </sst>
 </file>
@@ -410,7 +400,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,47 +414,47 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some files were checked and the script was further improved
</commit_message>
<xml_diff>
--- a/DataLoginFolder/dataLogin.xlsx
+++ b/DataLoginFolder/dataLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\eclipse-workspace\SwagLabs\DataLoginFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EE7FE0-FB9A-4A08-A0B1-1F69A993750B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3D2B47-5BE9-4CC4-99A5-6BDF25E4260F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{9DE631A4-C63C-460A-AE8C-CB17A0AD8551}"/>
   </bookViews>
@@ -25,27 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>standard_user</t>
   </si>
   <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
     <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -397,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D748CD72-7396-4F3F-A926-CD2104F758F8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,47 +399,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>